<commit_message>
Final submit met alle nieuwe documenten
</commit_message>
<xml_diff>
--- a/Documentatie/Product Backlog.xlsx
+++ b/Documentatie/Product Backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT BACKLOG" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="110">
   <si>
     <t>SPRINT 1 BACKLOG</t>
   </si>
@@ -979,10 +979,10 @@
   <dimension ref="A1:AI1005"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
+      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -991,9 +991,14 @@
     <col min="2" max="2" width="85.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" customWidth="1"/>
-    <col min="5" max="8" width="7" customWidth="1"/>
-    <col min="9" max="14" width="7.33203125" customWidth="1"/>
-    <col min="15" max="21" width="11.44140625" customWidth="1"/>
+    <col min="5" max="6" width="7" customWidth="1"/>
+    <col min="7" max="7" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" customWidth="1"/>
+    <col min="9" max="10" width="7.33203125" customWidth="1"/>
+    <col min="11" max="11" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="7.33203125" customWidth="1"/>
+    <col min="15" max="15" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="11.44140625" customWidth="1"/>
     <col min="22" max="35" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1347,9 +1352,11 @@
         <v>52</v>
       </c>
       <c r="N8" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="O8" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -1447,9 +1454,11 @@
         <v>52</v>
       </c>
       <c r="N10" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="O10" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -1496,9 +1505,11 @@
         <v>52</v>
       </c>
       <c r="N11" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="O11" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
@@ -1545,9 +1556,11 @@
         <v>52</v>
       </c>
       <c r="N12" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="O12" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -1594,9 +1607,11 @@
         <v>52</v>
       </c>
       <c r="N13" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="O13" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
@@ -1643,9 +1658,11 @@
         <v>52</v>
       </c>
       <c r="N14" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="O14" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -1692,9 +1709,11 @@
         <v>52</v>
       </c>
       <c r="N15" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="O15" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -38854,7 +38873,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>